<commit_message>
add images & fields
</commit_message>
<xml_diff>
--- a/data/meta/sf_displace_fields.xlsx
+++ b/data/meta/sf_displace_fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nelms\Documents\Penn\CPLN-680\Permit_Metrics\data\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71761B2F-FBD7-47B2-9279-AF5BBE47C905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC2853C-8635-403A-AD24-3D08B4E01FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="540" windowWidth="19420" windowHeight="10420" xr2:uid="{2B1BEE77-B50C-41C5-ABE0-0592596DE786}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2B1BEE77-B50C-41C5-ABE0-0592596DE786}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2167,9 +2167,6 @@
     <t>hh.tot.18</t>
   </si>
   <si>
-    <t>hinc.tot.18</t>
-  </si>
-  <si>
     <t>mhval.tot.18</t>
   </si>
   <si>
@@ -2606,6 +2603,9 @@
   </si>
   <si>
     <t>units.tot.90</t>
+  </si>
+  <si>
+    <t>hh_inc.med.18</t>
   </si>
 </sst>
 </file>
@@ -2656,16 +2656,6 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2697,6 +2687,16 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2711,13 +2711,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E88025BE-4C8D-4125-855C-D96A601DFA07}" name="Table1" displayName="Table1" ref="A1:D361" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="A1:D361" xr:uid="{E88025BE-4C8D-4125-855C-D96A601DFA07}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E88025BE-4C8D-4125-855C-D96A601DFA07}" name="Table1" displayName="Table1" ref="A1:D361" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:D361" xr:uid="{E88025BE-4C8D-4125-855C-D96A601DFA07}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="aboverm_pctch_real_hinc_00_18"/>
+        <filter val="aboverm_pctch_real_hinc_90_00"/>
+        <filter val="high_pdmt_medhhinc_00"/>
+        <filter val="high_pdmt_medhhinc_18"/>
+        <filter val="hinc_00"/>
+        <filter val="hinc_18"/>
+        <filter val="hinc_90"/>
+        <filter val="house_increase"/>
+        <filter val="house_rapid_increase"/>
+        <filter val="iinc_12"/>
+        <filter val="iinc_18"/>
+        <filter val="inc_cat_medhhinc_00"/>
+        <filter val="inc_cat_medhhinc_18"/>
+        <filter val="inc_cat_medhhinc_encoded00"/>
+        <filter val="inc_cat_medhhinc_encoded18"/>
+        <filter val="inc120_00"/>
+        <filter val="inc120_18"/>
+        <filter val="inc80_00"/>
+        <filter val="inc80_18"/>
+        <filter val="inc80_90"/>
+        <filter val="low_pdmt_medhhinc_00"/>
+        <filter val="low_pdmt_medhhinc_18"/>
+        <filter val="mix_high_medhhinc_00"/>
+        <filter val="mix_high_medhhinc_18"/>
+        <filter val="mix_low_medhhinc_00"/>
+        <filter val="mix_low_medhhinc_18"/>
+        <filter val="mix_mod_medhhinc_00"/>
+        <filter val="mix_mod_medhhinc_18"/>
+        <filter val="mod_pdmt_medhhinc_00"/>
+        <filter val="mod_pdmt_medhhinc_18"/>
+        <filter val="mov_fa_w_income_12"/>
+        <filter val="mov_fa_w_income_18"/>
+        <filter val="mov_oc_w_income_12"/>
+        <filter val="mov_oc_w_income_18"/>
+        <filter val="mov_os_w_income_12"/>
+        <filter val="mov_os_w_income_18"/>
+        <filter val="mov_tot_w_income_12"/>
+        <filter val="mov_tot_w_income_18"/>
+        <filter val="mov_wc_w_income_12"/>
+        <filter val="mov_wc_w_income_18"/>
+        <filter val="pctch_real_hinc_00_18"/>
+        <filter val="pctch_real_hinc_90_00"/>
+        <filter val="real_hinc_00"/>
+        <filter val="real_hinc_18"/>
+        <filter val="real_hinc_90"/>
+        <filter val="rent_increase"/>
+        <filter val="rent_rapid_increase"/>
+        <filter val="tot_increase"/>
+        <filter val="tot_rapid_increase"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:D274">
+    <sortCondition ref="A1:A361"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A4DA6248-EF18-46FC-8C22-7C5F0B9C24E1}" name="name" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{4EC703F0-B2DF-4319-BEBB-7D217180F7C8}" name="new" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A4DA6248-EF18-46FC-8C22-7C5F0B9C24E1}" name="name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4EC703F0-B2DF-4319-BEBB-7D217180F7C8}" name="new" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{F65A5719-A0BF-4A33-B61E-641A030F7C5E}" name="keep"/>
-    <tableColumn id="4" xr3:uid="{EF0ADD12-3761-495E-AA22-203FDFF1C5FA}" name="desc" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{EF0ADD12-3761-495E-AA22-203FDFF1C5FA}" name="desc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3022,8 +3079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0F88E8-2778-4509-8813-6A4699865B84}">
   <dimension ref="A1:D361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
-      <selection activeCell="D243" sqref="D243"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3046,12 +3103,12 @@
         <v>703</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C2" t="s">
         <v>705</v>
@@ -3060,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3074,7 +3131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3088,7 +3145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -3104,24 +3161,24 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>528</v>
       </c>
       <c r="B6" t="s">
-        <v>710</v>
+        <v>763</v>
       </c>
       <c r="C6" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="C7" t="s">
         <v>705</v>
@@ -3130,7 +3187,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -3141,12 +3198,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="C9" t="s">
         <v>705</v>
@@ -3155,7 +3212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -3166,12 +3223,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C11" t="s">
         <v>705</v>
@@ -3180,12 +3237,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C12" t="s">
         <v>706</v>
@@ -3194,12 +3251,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C13" t="s">
         <v>706</v>
@@ -3208,12 +3265,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C14" t="s">
         <v>706</v>
@@ -3222,12 +3279,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C15" t="s">
         <v>706</v>
@@ -3236,12 +3293,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C16" t="s">
         <v>706</v>
@@ -3250,12 +3307,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C17" t="s">
         <v>706</v>
@@ -3264,12 +3321,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C18" t="s">
         <v>706</v>
@@ -3278,12 +3335,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C19" t="s">
         <v>705</v>
@@ -3292,12 +3349,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C20" t="s">
         <v>705</v>
@@ -3306,12 +3363,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C21" t="s">
         <v>705</v>
@@ -3322,38 +3379,38 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>526</v>
       </c>
       <c r="B22" t="s">
-        <v>786</v>
+        <v>526</v>
       </c>
       <c r="C22" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>527</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>326</v>
       </c>
       <c r="B23" t="s">
-        <v>851</v>
+        <v>326</v>
       </c>
       <c r="C23" t="s">
         <v>706</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C24" t="s">
         <v>706</v>
@@ -3362,12 +3419,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C25" t="s">
         <v>706</v>
@@ -3376,12 +3433,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C26" t="s">
         <v>706</v>
@@ -3390,12 +3447,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C27" t="s">
         <v>706</v>
@@ -3404,12 +3461,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C28" t="s">
         <v>706</v>
@@ -3418,12 +3475,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C29" t="s">
         <v>706</v>
@@ -3432,12 +3489,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>56</v>
       </c>
       <c r="B30" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C30" t="s">
         <v>706</v>
@@ -3446,12 +3503,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>58</v>
       </c>
       <c r="B31" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C31" t="s">
         <v>706</v>
@@ -3462,24 +3519,24 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>305</v>
       </c>
       <c r="B32" t="s">
-        <v>805</v>
+        <v>738</v>
       </c>
       <c r="C32" t="s">
         <v>706</v>
       </c>
       <c r="D32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>62</v>
       </c>
       <c r="B33" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C33" t="s">
         <v>706</v>
@@ -3488,12 +3545,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C34" t="s">
         <v>706</v>
@@ -3502,12 +3559,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C35" t="s">
         <v>706</v>
@@ -3516,7 +3573,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -3530,7 +3587,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -3544,7 +3601,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -3558,12 +3615,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>74</v>
       </c>
       <c r="B39" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C39" t="s">
         <v>706</v>
@@ -3572,12 +3629,12 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="C40" t="s">
         <v>706</v>
@@ -3586,12 +3643,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="C41" t="s">
         <v>706</v>
@@ -3600,12 +3657,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C42" t="s">
         <v>706</v>
@@ -3614,12 +3671,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C43" t="s">
         <v>706</v>
@@ -3630,24 +3687,24 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>246</v>
       </c>
       <c r="B44" t="s">
-        <v>806</v>
+        <v>833</v>
       </c>
       <c r="C44" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="C45" t="s">
         <v>706</v>
@@ -3656,12 +3713,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C46" t="s">
         <v>706</v>
@@ -3670,12 +3727,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="C47" t="s">
         <v>706</v>
@@ -3684,12 +3741,12 @@
         <v>91</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C48" t="s">
         <v>706</v>
@@ -3698,12 +3755,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="C49" t="s">
         <v>706</v>
@@ -3712,12 +3769,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>96</v>
       </c>
       <c r="B50" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="C50" t="s">
         <v>706</v>
@@ -3726,12 +3783,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="C51" t="s">
         <v>706</v>
@@ -3740,12 +3797,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="C52" t="s">
         <v>706</v>
@@ -3756,24 +3813,24 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="B53" t="s">
-        <v>804</v>
+        <v>856</v>
       </c>
       <c r="C53" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D53" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>104</v>
       </c>
       <c r="B54" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="C54" t="s">
         <v>706</v>
@@ -3782,12 +3839,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>106</v>
       </c>
       <c r="B55" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C55" t="s">
         <v>706</v>
@@ -3796,12 +3853,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="C56" t="s">
         <v>706</v>
@@ -3810,12 +3867,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>110</v>
       </c>
       <c r="B57" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="C57" t="s">
         <v>706</v>
@@ -3824,12 +3881,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>112</v>
       </c>
       <c r="B58" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="C58" t="s">
         <v>706</v>
@@ -3838,12 +3895,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>114</v>
       </c>
       <c r="B59" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="C59" t="s">
         <v>706</v>
@@ -3852,12 +3909,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>116</v>
       </c>
       <c r="B60" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="C60" t="s">
         <v>706</v>
@@ -3866,12 +3923,12 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>118</v>
       </c>
       <c r="B61" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="C61" t="s">
         <v>706</v>
@@ -3880,7 +3937,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -3894,12 +3951,12 @@
         <v>121</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C63" t="s">
         <v>705</v>
@@ -3908,7 +3965,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>124</v>
       </c>
@@ -3922,12 +3979,12 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C65" t="s">
         <v>705</v>
@@ -3936,7 +3993,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>128</v>
       </c>
@@ -3952,19 +4009,19 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>130</v>
+        <v>274</v>
       </c>
       <c r="B67" t="s">
-        <v>800</v>
+        <v>839</v>
       </c>
       <c r="C67" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D67" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>132</v>
       </c>
@@ -3978,7 +4035,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -3992,7 +4049,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>136</v>
       </c>
@@ -4006,7 +4063,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>138</v>
       </c>
@@ -4020,7 +4077,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -4034,7 +4091,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>142</v>
       </c>
@@ -4048,7 +4105,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -4062,7 +4119,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>146</v>
       </c>
@@ -4078,19 +4135,19 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>425</v>
       </c>
       <c r="B76" t="s">
-        <v>801</v>
+        <v>425</v>
       </c>
       <c r="C76" t="s">
         <v>706</v>
       </c>
       <c r="D76" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -4104,7 +4161,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -4118,7 +4175,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>154</v>
       </c>
@@ -4132,7 +4189,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>156</v>
       </c>
@@ -4146,7 +4203,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>158</v>
       </c>
@@ -4160,7 +4217,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>160</v>
       </c>
@@ -4174,7 +4231,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>162</v>
       </c>
@@ -4188,7 +4245,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>164</v>
       </c>
@@ -4204,19 +4261,19 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>166</v>
+        <v>427</v>
       </c>
       <c r="B85" t="s">
-        <v>802</v>
+        <v>427</v>
       </c>
       <c r="C85" t="s">
         <v>706</v>
       </c>
       <c r="D85" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>168</v>
       </c>
@@ -4230,7 +4287,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>170</v>
       </c>
@@ -4244,7 +4301,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>172</v>
       </c>
@@ -4258,7 +4315,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>174</v>
       </c>
@@ -4272,7 +4329,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>176</v>
       </c>
@@ -4286,7 +4343,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>178</v>
       </c>
@@ -4300,7 +4357,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>180</v>
       </c>
@@ -4314,7 +4371,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>182</v>
       </c>
@@ -4330,19 +4387,19 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
       <c r="B94" t="s">
-        <v>803</v>
+        <v>829</v>
       </c>
       <c r="C94" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D94" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>186</v>
       </c>
@@ -4356,7 +4413,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -4370,7 +4427,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>190</v>
       </c>
@@ -4384,7 +4441,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>192</v>
       </c>
@@ -4398,7 +4455,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>194</v>
       </c>
@@ -4412,7 +4469,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>196</v>
       </c>
@@ -4426,7 +4483,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>198</v>
       </c>
@@ -4440,7 +4497,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>200</v>
       </c>
@@ -4456,24 +4513,24 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>202</v>
+        <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>830</v>
+        <v>785</v>
       </c>
       <c r="C103" t="s">
         <v>705</v>
       </c>
       <c r="D103" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>204</v>
       </c>
       <c r="B104" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C104" t="s">
         <v>705</v>
@@ -4482,12 +4539,12 @@
         <v>205</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>206</v>
       </c>
       <c r="B105" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C105" t="s">
         <v>705</v>
@@ -4496,12 +4553,12 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>208</v>
       </c>
       <c r="B106" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C106" t="s">
         <v>705</v>
@@ -4510,12 +4567,12 @@
         <v>209</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>210</v>
       </c>
       <c r="B107" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C107" t="s">
         <v>705</v>
@@ -4524,12 +4581,12 @@
         <v>211</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>212</v>
       </c>
       <c r="B108" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C108" t="s">
         <v>705</v>
@@ -4538,7 +4595,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>214</v>
       </c>
@@ -4549,7 +4606,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>216</v>
       </c>
@@ -4560,7 +4617,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>218</v>
       </c>
@@ -4571,7 +4628,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>220</v>
       </c>
@@ -4585,12 +4642,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>222</v>
       </c>
       <c r="B113" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C113" t="s">
         <v>706</v>
@@ -4599,12 +4656,12 @@
         <v>223</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>224</v>
       </c>
       <c r="B114" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C114" t="s">
         <v>706</v>
@@ -4613,12 +4670,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>226</v>
       </c>
       <c r="B115" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C115" t="s">
         <v>706</v>
@@ -4627,12 +4684,12 @@
         <v>227</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>228</v>
       </c>
       <c r="B116" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C116" t="s">
         <v>706</v>
@@ -4641,12 +4698,12 @@
         <v>229</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>230</v>
       </c>
       <c r="B117" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C117" t="s">
         <v>706</v>
@@ -4655,12 +4712,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>232</v>
       </c>
       <c r="B118" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C118" t="s">
         <v>706</v>
@@ -4669,12 +4726,12 @@
         <v>233</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>234</v>
       </c>
       <c r="B119" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C119" t="s">
         <v>706</v>
@@ -4683,12 +4740,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>236</v>
       </c>
       <c r="B120" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C120" t="s">
         <v>706</v>
@@ -4697,12 +4754,12 @@
         <v>237</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>238</v>
       </c>
       <c r="B121" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C121" t="s">
         <v>706</v>
@@ -4711,12 +4768,12 @@
         <v>239</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>240</v>
       </c>
       <c r="B122" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C122" t="s">
         <v>705</v>
@@ -4725,12 +4782,12 @@
         <v>241</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>242</v>
       </c>
       <c r="B123" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C123" t="s">
         <v>705</v>
@@ -4739,12 +4796,12 @@
         <v>243</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>244</v>
       </c>
       <c r="B124" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C124" t="s">
         <v>705</v>
@@ -4755,19 +4812,19 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>246</v>
+        <v>331</v>
       </c>
       <c r="B125" t="s">
-        <v>834</v>
+        <v>331</v>
       </c>
       <c r="C125" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D125" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>248</v>
       </c>
@@ -4781,12 +4838,12 @@
         <v>249</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>250</v>
       </c>
       <c r="B127" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C127" t="s">
         <v>705</v>
@@ -4795,12 +4852,12 @@
         <v>251</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>252</v>
       </c>
       <c r="B128" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C128" t="s">
         <v>705</v>
@@ -4809,12 +4866,12 @@
         <v>253</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>254</v>
       </c>
       <c r="B129" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C129" t="s">
         <v>705</v>
@@ -4823,7 +4880,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>256</v>
       </c>
@@ -4837,7 +4894,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>258</v>
       </c>
@@ -4851,7 +4908,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>260</v>
       </c>
@@ -4865,7 +4922,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>262</v>
       </c>
@@ -4879,7 +4936,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>264</v>
       </c>
@@ -4893,7 +4950,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>266</v>
       </c>
@@ -4907,7 +4964,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>268</v>
       </c>
@@ -4921,12 +4978,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>270</v>
       </c>
       <c r="B137" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C137" t="s">
         <v>705</v>
@@ -4935,12 +4992,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>272</v>
       </c>
       <c r="B138" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C138" t="s">
         <v>705</v>
@@ -4951,24 +5008,24 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>274</v>
+        <v>315</v>
       </c>
       <c r="B139" t="s">
-        <v>840</v>
+        <v>743</v>
       </c>
       <c r="C139" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D139" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>276</v>
       </c>
       <c r="B140" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C140" t="s">
         <v>705</v>
@@ -4977,12 +5034,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>278</v>
       </c>
       <c r="B141" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C141" t="s">
         <v>705</v>
@@ -4991,7 +5048,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>280</v>
       </c>
@@ -5005,7 +5062,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>281</v>
       </c>
@@ -5019,7 +5076,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>282</v>
       </c>
@@ -5033,7 +5090,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>283</v>
       </c>
@@ -5047,7 +5104,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>285</v>
       </c>
@@ -5063,80 +5120,80 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>287</v>
+        <v>332</v>
       </c>
       <c r="B147" t="s">
-        <v>841</v>
+        <v>332</v>
       </c>
       <c r="C147" t="s">
         <v>706</v>
       </c>
       <c r="D147" t="s">
-        <v>288</v>
+        <v>318</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>289</v>
+        <v>317</v>
       </c>
       <c r="B148" t="s">
-        <v>734</v>
+        <v>317</v>
       </c>
       <c r="C148" t="s">
         <v>706</v>
       </c>
       <c r="D148" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="B149" t="s">
-        <v>842</v>
+        <v>293</v>
       </c>
       <c r="C149" t="s">
         <v>706</v>
       </c>
       <c r="D149" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B150" t="s">
-        <v>293</v>
+        <v>733</v>
       </c>
       <c r="C150" t="s">
         <v>706</v>
       </c>
       <c r="D150" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B151" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="C151" t="s">
         <v>706</v>
       </c>
       <c r="D151" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>297</v>
       </c>
       <c r="B152" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C152" t="s">
         <v>706</v>
@@ -5145,12 +5202,12 @@
         <v>298</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>299</v>
       </c>
       <c r="B153" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C153" t="s">
         <v>706</v>
@@ -5159,12 +5216,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>301</v>
       </c>
       <c r="B154" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="C154" t="s">
         <v>706</v>
@@ -5175,72 +5232,72 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="B155" t="s">
-        <v>738</v>
+        <v>840</v>
       </c>
       <c r="C155" t="s">
         <v>706</v>
       </c>
       <c r="D155" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B156" t="s">
-        <v>739</v>
+        <v>842</v>
       </c>
       <c r="C156" t="s">
         <v>706</v>
       </c>
       <c r="D156" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="B157" t="s">
-        <v>740</v>
+        <v>325</v>
       </c>
       <c r="C157" t="s">
         <v>706</v>
       </c>
       <c r="D157" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B158" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="C158" t="s">
         <v>706</v>
       </c>
       <c r="D158" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>311</v>
+        <v>330</v>
       </c>
       <c r="B159" t="s">
-        <v>742</v>
+        <v>330</v>
       </c>
       <c r="C159" t="s">
         <v>706</v>
       </c>
       <c r="D159" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.3">
@@ -5248,7 +5305,7 @@
         <v>313</v>
       </c>
       <c r="B160" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C160" t="s">
         <v>706</v>
@@ -5259,33 +5316,33 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>315</v>
+        <v>328</v>
       </c>
       <c r="B161" t="s">
-        <v>744</v>
+        <v>328</v>
       </c>
       <c r="C161" t="s">
         <v>706</v>
       </c>
       <c r="D161" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B162" t="s">
-        <v>317</v>
+        <v>740</v>
       </c>
       <c r="C162" t="s">
         <v>706</v>
       </c>
       <c r="D162" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>319</v>
       </c>
@@ -5299,7 +5356,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>321</v>
       </c>
@@ -5313,7 +5370,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>323</v>
       </c>
@@ -5329,30 +5386,30 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="B166" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C166" t="s">
         <v>706</v>
       </c>
       <c r="D166" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="B167" t="s">
-        <v>326</v>
+        <v>741</v>
       </c>
       <c r="C167" t="s">
         <v>706</v>
       </c>
       <c r="D167" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.3">
@@ -5371,80 +5428,80 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
       <c r="B169" t="s">
-        <v>328</v>
+        <v>739</v>
       </c>
       <c r="C169" t="s">
         <v>706</v>
       </c>
       <c r="D169" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>329</v>
+        <v>184</v>
       </c>
       <c r="B170" t="s">
-        <v>329</v>
+        <v>802</v>
       </c>
       <c r="C170" t="s">
         <v>706</v>
       </c>
       <c r="D170" t="s">
-        <v>312</v>
+        <v>185</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>330</v>
+        <v>102</v>
       </c>
       <c r="B171" t="s">
-        <v>330</v>
+        <v>803</v>
       </c>
       <c r="C171" t="s">
         <v>706</v>
       </c>
       <c r="D171" t="s">
-        <v>314</v>
+        <v>103</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>331</v>
+        <v>148</v>
       </c>
       <c r="B172" t="s">
-        <v>331</v>
+        <v>800</v>
       </c>
       <c r="C172" t="s">
         <v>706</v>
       </c>
       <c r="D172" t="s">
-        <v>316</v>
+        <v>149</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>332</v>
+        <v>60</v>
       </c>
       <c r="B173" t="s">
-        <v>332</v>
+        <v>804</v>
       </c>
       <c r="C173" t="s">
         <v>706</v>
       </c>
       <c r="D173" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>333</v>
       </c>
       <c r="B174" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C174" t="s">
         <v>705</v>
@@ -5453,12 +5510,12 @@
         <v>334</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>335</v>
       </c>
       <c r="B175" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C175" t="s">
         <v>705</v>
@@ -5467,12 +5524,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>336</v>
       </c>
       <c r="B176" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C176" t="s">
         <v>705</v>
@@ -5481,7 +5538,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>337</v>
       </c>
@@ -5495,7 +5552,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>339</v>
       </c>
@@ -5509,12 +5566,12 @@
         <v>340</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>341</v>
       </c>
       <c r="B179" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C179" t="s">
         <v>706</v>
@@ -5523,7 +5580,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>343</v>
       </c>
@@ -5537,7 +5594,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>345</v>
       </c>
@@ -5553,19 +5610,19 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>347</v>
+        <v>166</v>
       </c>
       <c r="B182" t="s">
-        <v>347</v>
+        <v>801</v>
       </c>
       <c r="C182" t="s">
         <v>706</v>
       </c>
       <c r="D182" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>349</v>
       </c>
@@ -5579,7 +5636,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>351</v>
       </c>
@@ -5595,19 +5652,19 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>353</v>
+        <v>84</v>
       </c>
       <c r="B185" t="s">
-        <v>353</v>
+        <v>805</v>
       </c>
       <c r="C185" t="s">
         <v>706</v>
       </c>
       <c r="D185" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>355</v>
       </c>
@@ -5621,7 +5678,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>357</v>
       </c>
@@ -5635,12 +5692,12 @@
         <v>358</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>359</v>
       </c>
       <c r="B188" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C188" t="s">
         <v>706</v>
@@ -5649,12 +5706,12 @@
         <v>360</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>361</v>
       </c>
       <c r="B189" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C189" t="s">
         <v>706</v>
@@ -5665,19 +5722,19 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>363</v>
+        <v>403</v>
       </c>
       <c r="B190" t="s">
-        <v>748</v>
+        <v>851</v>
       </c>
       <c r="C190" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D190" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>365</v>
       </c>
@@ -5691,7 +5748,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>367</v>
       </c>
@@ -5705,12 +5762,12 @@
         <v>368</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>369</v>
       </c>
       <c r="B193" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C193" t="s">
         <v>706</v>
@@ -5719,12 +5776,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>371</v>
       </c>
       <c r="B194" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C194" t="s">
         <v>706</v>
@@ -5733,12 +5790,12 @@
         <v>372</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>373</v>
       </c>
       <c r="B195" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C195" t="s">
         <v>705</v>
@@ -5747,12 +5804,12 @@
         <v>374</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>375</v>
       </c>
       <c r="B196" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C196" t="s">
         <v>705</v>
@@ -5761,12 +5818,12 @@
         <v>376</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>377</v>
       </c>
       <c r="B197" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C197" t="s">
         <v>706</v>
@@ -5775,12 +5832,12 @@
         <v>378</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>379</v>
       </c>
       <c r="B198" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C198" t="s">
         <v>705</v>
@@ -5789,7 +5846,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>381</v>
       </c>
@@ -5803,7 +5860,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>383</v>
       </c>
@@ -5817,7 +5874,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>385</v>
       </c>
@@ -5831,7 +5888,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>387</v>
       </c>
@@ -5845,7 +5902,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>389</v>
       </c>
@@ -5859,7 +5916,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>391</v>
       </c>
@@ -5873,12 +5930,12 @@
         <v>392</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>393</v>
       </c>
       <c r="B205" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C205" t="s">
         <v>705</v>
@@ -5887,12 +5944,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>395</v>
       </c>
       <c r="B206" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C206" t="s">
         <v>706</v>
@@ -5901,12 +5958,12 @@
         <v>396</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>397</v>
       </c>
       <c r="B207" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C207" t="s">
         <v>706</v>
@@ -5920,7 +5977,7 @@
         <v>399</v>
       </c>
       <c r="B208" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C208" t="s">
         <v>705</v>
@@ -5929,12 +5986,12 @@
         <v>400</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>401</v>
       </c>
       <c r="B209" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C209" t="s">
         <v>706</v>
@@ -5945,19 +6002,19 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>403</v>
+        <v>130</v>
       </c>
       <c r="B210" t="s">
-        <v>852</v>
+        <v>799</v>
       </c>
       <c r="C210" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D210" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>405</v>
       </c>
@@ -5971,7 +6028,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>407</v>
       </c>
@@ -5985,12 +6042,12 @@
         <v>408</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>409</v>
       </c>
       <c r="B213" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C213" t="s">
         <v>705</v>
@@ -5999,12 +6056,12 @@
         <v>410</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>411</v>
       </c>
       <c r="B214" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C214" t="s">
         <v>705</v>
@@ -6013,7 +6070,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>413</v>
       </c>
@@ -6027,7 +6084,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>415</v>
       </c>
@@ -6043,33 +6100,33 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>417</v>
+        <v>42</v>
       </c>
       <c r="B217" t="s">
-        <v>417</v>
+        <v>850</v>
       </c>
       <c r="C217" t="s">
         <v>706</v>
       </c>
       <c r="D217" t="s">
-        <v>418</v>
+        <v>43</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>419</v>
+        <v>461</v>
       </c>
       <c r="B218" t="s">
-        <v>419</v>
+        <v>828</v>
       </c>
       <c r="C218" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D218" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>421</v>
       </c>
@@ -6083,7 +6140,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>423</v>
       </c>
@@ -6099,33 +6156,33 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c r="B221" t="s">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c r="C221" t="s">
         <v>706</v>
       </c>
       <c r="D221" t="s">
-        <v>426</v>
+        <v>458</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>427</v>
+        <v>353</v>
       </c>
       <c r="B222" t="s">
-        <v>427</v>
+        <v>353</v>
       </c>
       <c r="C222" t="s">
         <v>706</v>
       </c>
       <c r="D222" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>429</v>
       </c>
@@ -6139,7 +6196,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>431</v>
       </c>
@@ -6155,33 +6212,33 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>433</v>
+        <v>363</v>
       </c>
       <c r="B225" t="s">
-        <v>433</v>
+        <v>747</v>
       </c>
       <c r="C225" t="s">
         <v>706</v>
       </c>
       <c r="D225" t="s">
-        <v>434</v>
+        <v>364</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>435</v>
+        <v>347</v>
       </c>
       <c r="B226" t="s">
-        <v>435</v>
+        <v>347</v>
       </c>
       <c r="C226" t="s">
         <v>706</v>
       </c>
       <c r="D226" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>437</v>
       </c>
@@ -6195,7 +6252,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>439</v>
       </c>
@@ -6209,12 +6266,12 @@
         <v>438</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>440</v>
       </c>
       <c r="B229" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C229" t="s">
         <v>705</v>
@@ -6223,12 +6280,12 @@
         <v>441</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>442</v>
       </c>
       <c r="B230" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C230" t="s">
         <v>706</v>
@@ -6237,7 +6294,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>444</v>
       </c>
@@ -6251,12 +6308,12 @@
         <v>443</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>445</v>
       </c>
       <c r="B232" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C232" t="s">
         <v>706</v>
@@ -6265,7 +6322,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>447</v>
       </c>
@@ -6279,7 +6336,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>449</v>
       </c>
@@ -6293,7 +6350,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>451</v>
       </c>
@@ -6307,7 +6364,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>453</v>
       </c>
@@ -6321,7 +6378,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>455</v>
       </c>
@@ -6337,24 +6394,24 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="B238" t="s">
-        <v>457</v>
+        <v>417</v>
       </c>
       <c r="C238" t="s">
         <v>706</v>
       </c>
       <c r="D238" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>459</v>
       </c>
       <c r="B239" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C239" t="s">
         <v>706</v>
@@ -6365,19 +6422,19 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>461</v>
+        <v>419</v>
       </c>
       <c r="B240" t="s">
-        <v>829</v>
+        <v>419</v>
       </c>
       <c r="C240" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="D240" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>463</v>
       </c>
@@ -6391,12 +6448,12 @@
         <v>464</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>465</v>
       </c>
       <c r="B242" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C242" t="s">
         <v>706</v>
@@ -6405,7 +6462,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>467</v>
       </c>
@@ -6419,12 +6476,12 @@
         <v>468</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>469</v>
       </c>
       <c r="B244" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C244" t="s">
         <v>705</v>
@@ -6433,12 +6490,12 @@
         <v>470</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>471</v>
       </c>
       <c r="B245" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C245" t="s">
         <v>706</v>
@@ -6447,7 +6504,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>473</v>
       </c>
@@ -6461,7 +6518,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>475</v>
       </c>
@@ -6475,7 +6532,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>477</v>
       </c>
@@ -6489,12 +6546,12 @@
         <v>478</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>479</v>
       </c>
       <c r="B249" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C249" t="s">
         <v>706</v>
@@ -6503,12 +6560,12 @@
         <v>480</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>481</v>
       </c>
       <c r="B250" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C250" t="s">
         <v>706</v>
@@ -6517,7 +6574,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>483</v>
       </c>
@@ -6531,7 +6588,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>485</v>
       </c>
@@ -6545,7 +6602,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>487</v>
       </c>
@@ -6559,7 +6616,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>489</v>
       </c>
@@ -6573,12 +6630,12 @@
         <v>490</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>491</v>
       </c>
       <c r="B255" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C255" t="s">
         <v>706</v>
@@ -6587,7 +6644,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>493</v>
       </c>
@@ -6601,7 +6658,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>495</v>
       </c>
@@ -6615,12 +6672,12 @@
         <v>496</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>497</v>
       </c>
       <c r="B258" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C258" t="s">
         <v>706</v>
@@ -6629,7 +6686,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>499</v>
       </c>
@@ -6643,7 +6700,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>501</v>
       </c>
@@ -6657,7 +6714,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>503</v>
       </c>
@@ -6671,12 +6728,12 @@
         <v>504</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>505</v>
       </c>
       <c r="B262" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C262" t="s">
         <v>706</v>
@@ -6685,7 +6742,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>507</v>
       </c>
@@ -6699,7 +6756,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>509</v>
       </c>
@@ -6713,12 +6770,12 @@
         <v>510</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>511</v>
       </c>
       <c r="B265" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C265" t="s">
         <v>706</v>
@@ -6727,12 +6784,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>513</v>
       </c>
       <c r="B266" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C266" t="s">
         <v>706</v>
@@ -6741,12 +6798,12 @@
         <v>514</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>515</v>
       </c>
       <c r="B267" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C267" t="s">
         <v>706</v>
@@ -6755,12 +6812,12 @@
         <v>516</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>517</v>
       </c>
       <c r="B268" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C268" t="s">
         <v>706</v>
@@ -6769,7 +6826,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>519</v>
       </c>
@@ -6783,7 +6840,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>521</v>
       </c>
@@ -6797,7 +6854,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>522</v>
       </c>
@@ -6811,12 +6868,12 @@
         <v>523</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>524</v>
       </c>
       <c r="B272" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C272" t="s">
         <v>706</v>
@@ -6827,33 +6884,33 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>526</v>
+        <v>433</v>
       </c>
       <c r="B273" t="s">
-        <v>526</v>
+        <v>433</v>
       </c>
       <c r="C273" t="s">
         <v>706</v>
       </c>
       <c r="D273" t="s">
-        <v>527</v>
+        <v>434</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>528</v>
+        <v>435</v>
       </c>
       <c r="B274" t="s">
-        <v>764</v>
+        <v>435</v>
       </c>
       <c r="C274" t="s">
         <v>706</v>
       </c>
       <c r="D274" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>530</v>
       </c>
@@ -6867,12 +6924,12 @@
         <v>531</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>532</v>
       </c>
       <c r="B276" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C276" t="s">
         <v>706</v>
@@ -6881,12 +6938,12 @@
         <v>533</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>534</v>
       </c>
       <c r="B277" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C277" t="s">
         <v>706</v>
@@ -6895,7 +6952,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>536</v>
       </c>
@@ -6909,7 +6966,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>538</v>
       </c>
@@ -6923,7 +6980,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="280" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>540</v>
       </c>
@@ -6937,7 +6994,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="281" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>542</v>
       </c>
@@ -6951,12 +7008,12 @@
         <v>543</v>
       </c>
     </row>
-    <row r="282" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>544</v>
       </c>
       <c r="B282" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C282" t="s">
         <v>706</v>
@@ -6965,7 +7022,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="283" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>546</v>
       </c>
@@ -6979,12 +7036,12 @@
         <v>547</v>
       </c>
     </row>
-    <row r="284" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>548</v>
       </c>
       <c r="B284" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C284" t="s">
         <v>706</v>
@@ -6993,7 +7050,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="285" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>550</v>
       </c>
@@ -7007,7 +7064,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="286" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>552</v>
       </c>
@@ -7021,12 +7078,12 @@
         <v>553</v>
       </c>
     </row>
-    <row r="287" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>554</v>
       </c>
       <c r="B287" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C287" t="s">
         <v>706</v>
@@ -7035,12 +7092,12 @@
         <v>555</v>
       </c>
     </row>
-    <row r="288" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>556</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C288" t="s">
         <v>706</v>
@@ -7049,7 +7106,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="289" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>557</v>
       </c>
@@ -7063,7 +7120,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="290" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>558</v>
       </c>
@@ -7077,7 +7134,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="291" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>560</v>
       </c>
@@ -7091,7 +7148,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="292" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>562</v>
       </c>
@@ -7105,7 +7162,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="293" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>564</v>
       </c>
@@ -7119,7 +7176,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="294" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>566</v>
       </c>
@@ -7133,7 +7190,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="295" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>568</v>
       </c>
@@ -7147,7 +7204,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="296" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>570</v>
       </c>
@@ -7161,7 +7218,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="297" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" s="1" t="s">
         <v>572</v>
       </c>
@@ -7175,7 +7232,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="298" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" s="1" t="s">
         <v>574</v>
       </c>
@@ -7189,7 +7246,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="299" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" s="1" t="s">
         <v>576</v>
       </c>
@@ -7203,7 +7260,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="300" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" s="1" t="s">
         <v>578</v>
       </c>
@@ -7217,7 +7274,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="301" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" s="1" t="s">
         <v>580</v>
       </c>
@@ -7231,7 +7288,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="302" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" s="1" t="s">
         <v>582</v>
       </c>
@@ -7245,7 +7302,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="303" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" s="1" t="s">
         <v>584</v>
       </c>
@@ -7259,7 +7316,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="304" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" s="1" t="s">
         <v>586</v>
       </c>
@@ -7273,7 +7330,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="305" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" s="1" t="s">
         <v>588</v>
       </c>
@@ -7287,7 +7344,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="306" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" s="1" t="s">
         <v>590</v>
       </c>
@@ -7301,7 +7358,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="307" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" s="1" t="s">
         <v>591</v>
       </c>
@@ -7315,7 +7372,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="308" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" s="1" t="s">
         <v>593</v>
       </c>
@@ -7329,7 +7386,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="309" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" s="1" t="s">
         <v>595</v>
       </c>
@@ -7343,7 +7400,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="310" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" s="1" t="s">
         <v>597</v>
       </c>
@@ -7357,7 +7414,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="311" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" s="1" t="s">
         <v>599</v>
       </c>
@@ -7371,7 +7428,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="312" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" s="1" t="s">
         <v>601</v>
       </c>
@@ -7385,7 +7442,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="313" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" s="1" t="s">
         <v>603</v>
       </c>
@@ -7399,7 +7456,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="314" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" s="1" t="s">
         <v>605</v>
       </c>
@@ -7413,7 +7470,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="315" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" s="1" t="s">
         <v>607</v>
       </c>
@@ -7427,7 +7484,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="316" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A316" s="1" t="s">
         <v>609</v>
       </c>
@@ -7441,7 +7498,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="317" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" s="1" t="s">
         <v>611</v>
       </c>
@@ -7455,7 +7512,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="318" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" s="1" t="s">
         <v>613</v>
       </c>
@@ -7469,7 +7526,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="319" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" s="1" t="s">
         <v>615</v>
       </c>
@@ -7483,7 +7540,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="320" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" s="1" t="s">
         <v>617</v>
       </c>
@@ -7497,7 +7554,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="321" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" s="1" t="s">
         <v>619</v>
       </c>
@@ -7511,7 +7568,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="322" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" s="1" t="s">
         <v>621</v>
       </c>
@@ -7525,7 +7582,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="323" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" s="1" t="s">
         <v>623</v>
       </c>
@@ -7539,7 +7596,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="324" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" s="1" t="s">
         <v>625</v>
       </c>
@@ -7553,7 +7610,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="325" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" s="1" t="s">
         <v>627</v>
       </c>
@@ -7567,7 +7624,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="326" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" s="1" t="s">
         <v>629</v>
       </c>
@@ -7581,7 +7638,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="327" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" s="1" t="s">
         <v>631</v>
       </c>
@@ -7595,7 +7652,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="328" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" s="1" t="s">
         <v>633</v>
       </c>
@@ -7609,7 +7666,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="329" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" s="1" t="s">
         <v>635</v>
       </c>
@@ -7623,7 +7680,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="330" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" s="1" t="s">
         <v>637</v>
       </c>
@@ -7637,7 +7694,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="331" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" s="1" t="s">
         <v>639</v>
       </c>
@@ -7651,7 +7708,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="332" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" s="1" t="s">
         <v>641</v>
       </c>
@@ -7665,7 +7722,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="333" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" s="1" t="s">
         <v>643</v>
       </c>
@@ -7679,7 +7736,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="334" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" s="1" t="s">
         <v>645</v>
       </c>
@@ -7693,7 +7750,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="335" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" s="1" t="s">
         <v>647</v>
       </c>
@@ -7707,7 +7764,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="336" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" s="1" t="s">
         <v>649</v>
       </c>
@@ -7721,7 +7778,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="337" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A337" s="1" t="s">
         <v>651</v>
       </c>
@@ -7735,7 +7792,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="338" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A338" s="1" t="s">
         <v>653</v>
       </c>
@@ -7749,7 +7806,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="339" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A339" s="1" t="s">
         <v>655</v>
       </c>
@@ -7763,7 +7820,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="340" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A340" s="1" t="s">
         <v>657</v>
       </c>
@@ -7777,7 +7834,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="341" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A341" s="1" t="s">
         <v>659</v>
       </c>
@@ -7791,7 +7848,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="342" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A342" s="1" t="s">
         <v>661</v>
       </c>
@@ -7805,7 +7862,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="343" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A343" s="1" t="s">
         <v>663</v>
       </c>
@@ -7819,7 +7876,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="344" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A344" s="1" t="s">
         <v>665</v>
       </c>
@@ -7833,7 +7890,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="345" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A345" s="1" t="s">
         <v>666</v>
       </c>
@@ -7847,7 +7904,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="346" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A346" s="1" t="s">
         <v>667</v>
       </c>
@@ -7861,7 +7918,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="347" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A347" s="1" t="s">
         <v>668</v>
       </c>
@@ -7875,7 +7932,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="348" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A348" s="1" t="s">
         <v>669</v>
       </c>
@@ -7889,7 +7946,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="349" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A349" s="1" t="s">
         <v>670</v>
       </c>
@@ -7903,7 +7960,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="350" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A350" s="1" t="s">
         <v>672</v>
       </c>
@@ -7917,7 +7974,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="351" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A351" s="1" t="s">
         <v>674</v>
       </c>
@@ -7931,7 +7988,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="352" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A352" s="1" t="s">
         <v>676</v>
       </c>
@@ -7945,7 +8002,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="353" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A353" s="1" t="s">
         <v>678</v>
       </c>
@@ -7959,7 +8016,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="354" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A354" s="1" t="s">
         <v>680</v>
       </c>
@@ -7973,12 +8030,12 @@
         <v>681</v>
       </c>
     </row>
-    <row r="355" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A355" s="1" t="s">
         <v>682</v>
       </c>
       <c r="B355" s="1" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C355" t="s">
         <v>706</v>
@@ -7987,12 +8044,12 @@
         <v>683</v>
       </c>
     </row>
-    <row r="356" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A356" s="1" t="s">
         <v>684</v>
       </c>
       <c r="B356" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C356" t="s">
         <v>706</v>
@@ -8001,12 +8058,12 @@
         <v>683</v>
       </c>
     </row>
-    <row r="357" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A357" s="1" t="s">
         <v>685</v>
       </c>
       <c r="B357" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C357" t="s">
         <v>706</v>
@@ -8015,12 +8072,12 @@
         <v>686</v>
       </c>
     </row>
-    <row r="358" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A358" s="1" t="s">
         <v>687</v>
       </c>
       <c r="B358" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C358" t="s">
         <v>706</v>
@@ -8029,7 +8086,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="359" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A359" s="1" t="s">
         <v>689</v>
       </c>
@@ -8043,7 +8100,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="360" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A360" s="1" t="s">
         <v>691</v>
       </c>
@@ -8057,7 +8114,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="361" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:4" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A361" s="1" t="s">
         <v>693</v>
       </c>
@@ -8073,7 +8130,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>